<commit_message>
updated README and added NCBI upload metadata
</commit_message>
<xml_diff>
--- a/TagSeq/Analysis/Output/MS_materials/Tables/KEGG_summary.xlsx
+++ b/TagSeq/Analysis/Output/MS_materials/Tables/KEGG_summary.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\My_Projects\Pgenerosa_TagSeq_Metabolomics\TagSeq\Analysis\Output\MS_materials\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8982D8D-7D8A-4D02-817D-B65254917F37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B9B8E1-A003-4C2E-8AEA-AB0661BDE615}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="180" windowWidth="18000" windowHeight="9360" xr2:uid="{10F09BC0-F421-4E18-B283-2FBE16DB1E0F}"/>
+    <workbookView xWindow="-28920" yWindow="-10305" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{10F09BC0-F421-4E18-B283-2FBE16DB1E0F}"/>
   </bookViews>
   <sheets>
     <sheet name="WGCNA_all_treatments" sheetId="5" r:id="rId1"/>
     <sheet name="DESeq2_MainEffects" sheetId="4" r:id="rId2"/>
+    <sheet name="WGCNA_subseq_exposures" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="99">
   <si>
     <t>Day7</t>
   </si>
@@ -578,6 +579,180 @@
   </si>
   <si>
     <t>Glycolysis / Gluconeogenesis</t>
+  </si>
+  <si>
+    <t>turquoise</t>
+  </si>
+  <si>
+    <t>greenyellow</t>
+  </si>
+  <si>
+    <t>Phagosome</t>
+  </si>
+  <si>
+    <t>Autophagy - animal</t>
+  </si>
+  <si>
+    <t>FoxO signaling pathway</t>
+  </si>
+  <si>
+    <t>Ribosome</t>
+  </si>
+  <si>
+    <t>Oxidative phosphorylation</t>
+  </si>
+  <si>
+    <r>
+      <t>1343</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (957)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1495 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1023)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1126 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(808)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1776 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1243)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">532 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(385)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1554 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1140)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">664 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(451)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">448 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(316)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">827 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(570)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">956 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(707)</t>
+    </r>
+  </si>
+  <si>
+    <t>84 ± 3</t>
   </si>
 </sst>
 </file>
@@ -711,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -814,6 +989,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1130,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2985AB-8715-49D6-8A13-9A5F5ED7C8B7}">
   <dimension ref="A2:I62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A62" sqref="A60:XFD62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2716,4 +2896,875 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B51E910-7DBE-451A-A47D-2157280D197C}">
+  <dimension ref="A2:I50"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.42578125" style="1" customWidth="1"/>
+    <col min="11" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="14.85546875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="1:9" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="21"/>
+      <c r="C5" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:9" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="32"/>
+    </row>
+    <row r="9" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="33"/>
+      <c r="B9" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="32">
+        <v>85</v>
+      </c>
+      <c r="F9" s="43">
+        <v>4.0094409563064599E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>7</v>
+      </c>
+      <c r="H9" s="43">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="I9" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="33"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="43">
+        <v>4.0094409563064599E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>12</v>
+      </c>
+      <c r="H10" s="43">
+        <v>0.125</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="33"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="43">
+        <v>4.0094409563064599E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>12</v>
+      </c>
+      <c r="H11" s="43">
+        <v>0.12</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="33"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="43">
+        <v>1.67111411150558E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="43">
+        <v>0.112994350282486</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="33"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="43">
+        <v>2.3237806013084301E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="43">
+        <v>0.104712041884817</v>
+      </c>
+      <c r="I13" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="33"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="33"/>
+    </row>
+    <row r="15" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="33"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="32">
+        <v>83.7</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="1">
+        <v>20</v>
+      </c>
+      <c r="H15" s="43">
+        <v>0.18181818181818199</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="33"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="43">
+        <v>4.3313156320520699E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>9</v>
+      </c>
+      <c r="H16" s="43">
+        <v>0.163636363636364</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="33"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="43">
+        <v>4.3313156320520699E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>11</v>
+      </c>
+      <c r="H17" s="43">
+        <v>0.139240506329114</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="33"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="43">
+        <v>4.3313156320520699E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>19</v>
+      </c>
+      <c r="H18" s="43">
+        <v>0.10734463276836199</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="33"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="33"/>
+    </row>
+    <row r="20" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="33"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="32">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1">
+        <v>53</v>
+      </c>
+      <c r="H20" s="43">
+        <v>0.37323943661971798</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="33"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="43">
+        <v>8.8556606264046309E-3</v>
+      </c>
+      <c r="G21" s="1">
+        <v>19</v>
+      </c>
+      <c r="H21" s="43">
+        <v>0.19387755102040799</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="33"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="32"/>
+    </row>
+    <row r="23" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="33"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="32">
+        <v>87.6</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="33"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="38"/>
+    </row>
+    <row r="25" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="33"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="33"/>
+      <c r="B26" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="32">
+        <v>86.6</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="1">
+        <v>35</v>
+      </c>
+      <c r="H26" s="43">
+        <v>0.24647887323943701</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="33"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="43">
+        <v>2.1486896348554E-2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>21</v>
+      </c>
+      <c r="H27" s="43">
+        <v>0.17948717948717899</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="33"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="43">
+        <v>9.9236822101861997E-3</v>
+      </c>
+      <c r="G28" s="1">
+        <v>30</v>
+      </c>
+      <c r="H28" s="43">
+        <v>0.169491525423729</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="33"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="43">
+        <v>1.15774346008693E-2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>31</v>
+      </c>
+      <c r="H29" s="43">
+        <v>0.162303664921466</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="33"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="33"/>
+    </row>
+    <row r="31" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="33"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="32">
+        <v>81.3</v>
+      </c>
+      <c r="F31" s="43">
+        <v>9.1911822627132299E-4</v>
+      </c>
+      <c r="G31" s="1">
+        <v>12</v>
+      </c>
+      <c r="H31" s="43">
+        <v>0.122448979591837</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="33"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="38"/>
+    </row>
+    <row r="33" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="33"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="32"/>
+    </row>
+    <row r="34" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="33"/>
+      <c r="B34" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="32">
+        <v>87.8</v>
+      </c>
+      <c r="F34" s="43">
+        <v>1.16005770165034E-2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>8</v>
+      </c>
+      <c r="H34" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="I34" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="33"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="43">
+        <v>1.16005770165034E-2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>10</v>
+      </c>
+      <c r="H35" s="43">
+        <v>0.169491525423729</v>
+      </c>
+      <c r="I35" s="33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="33"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="43">
+        <v>4.3335548273475202E-3</v>
+      </c>
+      <c r="G36" s="1">
+        <v>15</v>
+      </c>
+      <c r="H36" s="43">
+        <v>0.15</v>
+      </c>
+      <c r="I36" s="33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="33"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="43">
+        <v>1.22480573074194E-2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>13</v>
+      </c>
+      <c r="H37" s="43">
+        <v>0.13541666666666699</v>
+      </c>
+      <c r="I37" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="33"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="43">
+        <v>5.0041186994384198E-4</v>
+      </c>
+      <c r="G38" s="1">
+        <v>25</v>
+      </c>
+      <c r="H38" s="43">
+        <v>0.130890052356021</v>
+      </c>
+      <c r="I38" s="33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="33"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="43">
+        <v>4.3335548273475202E-3</v>
+      </c>
+      <c r="G39" s="1">
+        <v>21</v>
+      </c>
+      <c r="H39" s="43">
+        <v>0.11864406779661001</v>
+      </c>
+      <c r="I39" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="33"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="33"/>
+    </row>
+    <row r="41" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="33"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="32">
+        <v>81.2</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="1">
+        <v>45</v>
+      </c>
+      <c r="H41" s="43">
+        <v>0.31690140845070403</v>
+      </c>
+      <c r="I41" s="33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="33"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="46">
+        <v>8.6520543401929998E-3</v>
+      </c>
+      <c r="G42" s="3">
+        <v>13</v>
+      </c>
+      <c r="H42" s="46">
+        <v>0.13265306122449</v>
+      </c>
+      <c r="I42" s="32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="33"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="32"/>
+    </row>
+    <row r="44" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="33"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" s="32">
+        <v>85</v>
+      </c>
+      <c r="F44" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="33"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="32"/>
+    </row>
+    <row r="46" spans="1:9" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="33"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" s="32">
+        <v>82</v>
+      </c>
+      <c r="F46" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="5" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="33"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="44"/>
+    </row>
+    <row r="48" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="33"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
+    </row>
+    <row r="49" spans="2:9" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+    </row>
+    <row r="50" spans="2:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>